<commit_message>
updated to generate level 1 and level 2 html
</commit_message>
<xml_diff>
--- a/togaf/data/conformance.xlsx
+++ b/togaf/data/conformance.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Level 1" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Level 2" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="323">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="696" uniqueCount="514">
   <si>
     <t xml:space="preserve">Level/Unit</t>
   </si>
@@ -1052,6 +1053,1057 @@
   <si>
     <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/architecture-content/chap04.html#tag_04_02_20</t>
   </si>
+  <si>
+    <t xml:space="preserve">Bloom"s Taxonomy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit 1 - The Context for EA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain why guiding effective change is the purpose of Enterprise Architecture.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G186 §3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_3.html#_Toc95288808</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain what an Enterprise Architecture looks like.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G186 §3.2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_3.html#_Toc95288812</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain what an Architecture Capability is.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S0} §3.13
+G184 §3.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/introduction/chap03.html#tag_03_13
+https://pubs.opengroup.org/togaf-standard/togaf-leaders-guide/togaf-leaders-guide_3.html#_Toc95220345</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the role of Architecture Governance and the role of an enterprise architect.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G186 §15.1
+G20F §4.4.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_15.html#_Toc95288919
+https://pubs.opengroup.org/togaf-standard/guides/enabling-enterprise-agility/index.html#_governance_in_architecture_iterations</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain Architecture Compliance, levels of conformance, reviews, and the role of the architect using the TOGAF diagram and the checklists from G186</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S5} §6.1, 6.2, 6.3
+G186 §15.2.1, 15.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/ea-capability-and-governance/chap06.html#tag_06_01
+https://pubs.opengroup.org/togaf-standard/ea-capability-and-governance/chap06.html#tag_06_02
+https://pubs.opengroup.org/togaf-standard/ea-capability-and-governance/chap06.html#tag_06_03
+https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_15.html#_Toc95288923
+https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_15.html#_Toc95288924</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how an architecture enables alignment to organizational objectives using Agile development as an example.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G186 §12.1, 11.4
+G20F §4.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_12.html#_Toc95288909
+https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_11.html#_Toc95288907
+https://pubs.opengroup.org/togaf-standard/guides/enabling-enterprise-agility/index.html#_adm_levels_and_phases_mapped_to_agile_concepts</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the need to manage multiple architecture states (e.g., candidate, current, transition, target).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G186 §5.4, 13</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_5.html#_Toc95288842
+https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_13.html#_Toc95288913</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Briefly explain Enterprise Security Architecture.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G152 §1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/integrating-risk-and-security/integrating-risk-and-security_1.html#_Toc95208526</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how security is a cross-cutting concern.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G152 §4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/integrating-risk-and-security/integrating-risk-and-security_4.html#_Toc95208548</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain why it is important to create an environment in which uncertainty of the success of change can be managed to optimize maximum business benefit and minimum business loss.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G152 §3.1.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/integrating-risk-and-security/integrating-risk-and-security_3.html#_Toc95208541</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Briefly explain the role of the Enterprise Architect and Enterprise Architecture in a Digital enterprise for four contexts of the DPBoK Standard.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G217 §4.2.1, 4.2.2, 4.2.3, 4.2.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/guides/using-the-togaf-standard-in-the-digital-enterprise/index.html#_context_i_individualfounder
+https://pubs.opengroup.org/togaf-standard/guides/using-the-togaf-standard-in-the-digital-enterprise/index.html#_context_ii_team
+https://pubs.opengroup.org/togaf-standard/guides/using-the-togaf-standard-in-the-digital-enterprise/index.html#_context_iii_team_of_teams
+https://pubs.opengroup.org/togaf-standard/guides/using-the-togaf-standard-in-the-digital-enterprise/index.html#_context_iv_enduring_enterprise</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit 2 - Stakeholder Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how to identify stakeholders, their concerns, views, and the communication involved.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">3_Applying</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G186 §3.3.1, B
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_3.html#_Toc95288814
+https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_15.html#_Toc95288929</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the use of architecture views.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S4} §3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how to manage stakeholders’ engagement and requirements.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how to use trade-off to support the architecture development.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S2} §10.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit 3 - Phase A, the Starting Point</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how to identify the information necessary to execute the Architecture Vision phase and how iteration cycles will provide more information to take into account in order to execute the phase.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §3.2
+G186 §5.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/adm/chap03.html#tag_03_02
+https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_5.html#_Toc95288833</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how to apply the phase and how it contributes to the architecture development work:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Scope of the Architecture Project</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §3.3
+G186 §5.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/adm/chap03.html#tag_03_03_06
+https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_5.html#_Toc95288833</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Stakeholders, their concerns, and business requirements</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/adm/chap03.html#tag_03_03_02
+https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_5.html#_Toc95288833</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Business goals, business drivers, and constraints</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/adm/chap03.html#tag_03_03_03
+https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_5.html#_Toc95288833</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe a security-specific architecture design to be carried out that is sufficient.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G152 §5.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the outputs necessary to proceed with the architecture development work:</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Statement of Architecture Work</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §3.4 
+{S4} §4.2
+G186 §5.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/adm/chap03.html#tag_03_04
+https://pubs.opengroup.org/togaf-standard/architecture-content/chap04.html#tag_04_02_20
+https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_5.html#_Toc95288834</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Architecture Vision</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/adm/chap03.html#tag_03_04
+https://pubs.opengroup.org/togaf-standard/architecture-content/chap04.html#tag_04_02_08
+https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_5.html#_Toc95288833
+</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Communications Plan</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">https://pubs.opengroup.org/togaf-standard/adm/chap03.html#tag_03_04
+https://pubs.opengroup.org/togaf-standard/architecture-content/chap04.html#tag_04_02_12
+https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_5.html#_Toc95288833</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit 4 - Architecture Development</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the steps applicable to all phases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G186 §6.3 (including §6.3.1-6.3.6)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain risk and security considerations during the architecture development.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G152 §5.3, 5.4, 5.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the information that is relevant to produce outputs valuable to the architecture development:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §4.2
+{S4} §4.2.9
+G186 §5.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">·     Business principles</t>
+  </si>
+  <si>
+    <t xml:space="preserve">·     Business goals</t>
+  </si>
+  <si>
+    <t xml:space="preserve">·     Business drivers</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how to apply Phase B and how it contributes to the architecture development work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §4.3
+G186 §5.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the information that is relevant to Phase C (Data and Applications) to produce outputs relevant to the architecture development.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §6.2, 7.2
+G186 §5.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how to apply Phase C and how it contributes to the architecture development work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §6.5, 7.5
+G186 §5.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the information needed in Phase D to produce outputs relevant to the architecture development.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §8.2
+G186 §5.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how to apply Phase D and how it contributes to the architecture development work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §8.5
+G186 §5.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the outputs of Phases B, C, and D necessary to proceed with the architecture development work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §4.4, 6.4, 7.4, 8.4
+G186 §5.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit 5 - Implementing the Architecture</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the risk and security considerations for the three Phases (E, F, and G).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G152 §5.6, 5.7, 5.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe the steps (Phase E) to create the Implementation and Migration Strategy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §9.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe three basic approaches to implementation.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §9.3.8</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how to identify and group work packages.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how to create and document Transition Architectures.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the impact of the migration projects on the organization and the coordination required.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §10.3
+G186 §5.2.2, 9, 10.4, 10.6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain why and how business value is assigned to each work package.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §10.3.2
+G186 §3.4, 9.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe how to prioritize the migration projects (Phase F).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §10.3.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe how to confirm the Architecture Roadmap (Phase F).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §10.3.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">5.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the outputs necessary to proceed with the architecture implementation work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §10.4
+G186 §5.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the inputs to Phase G.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §11.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how the Implementation Governance is executed (Phase G).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §11.3
+G186 §11.4, 15.1.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the outputs necessary to support Architecture Governance.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §11.4
+G186 §5.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how Architecture Contracts are used to communicate with implementers.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S5} §5.2
+G186 §3.3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how to balance opportunity and viability.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G186 §8.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit 6 - Architecture Change Management</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the inputs triggering change management:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §12.2
+{S4} 4.2.11
+G186 §14</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Change Requests</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the activities necessary for effective change management (Stakeholder Management).</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §12.3
+G186 §14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the outputs relevant to proceed.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §12.4
+G186 §5.2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit 7 - Requirements Mgt</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the inputs that can feed the Requirements Management phase.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">{S1} §13.2
+</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="&#10;G186 §6.1.1, 6.1.2"/>
+        <family val="0"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">G186 §6.1.1, 6.1.2</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how the Requirements Management steps correspond to ADM phase steps.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §13.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the purpose of the outputs of Requirements Management.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §13.4, {S4} §4.2.6, 4.2.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Unit 8 - Supporting the ADM work</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe how The Open Group TOGAF Library can be used to support the practitioner’s work.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S0} §2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Briefly explain the business scenario technique.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G176 §1, 3.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the purpose of compliance assessments.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S5} §6.3.1
+G186 §5.1.5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how migration planning techniques are used to review and consolidate the gap analysis results from earlier phases.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S2} §6</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe how a repository can be structured using the TOGAF repository as an example:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S4} §7.2, 7.3, 7.4, 7.5, 7.6, 7.7, 7.8</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Architecture Landscape</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Reference Library</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Standards Library</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Governance Repository</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Architecture Requirements Repository</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Solutions Landscape</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Enterprise Repository</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain what to expect in a well-run Architecture Repository.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G186 §5.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how the concepts of Architecture Levels are used to organize the Architecture Landscape.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S3} §3.1, 3.2, 3.3, 3.4</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the different levels of architecture that exist in an organization.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain at which level an architecture is being developed and the associated level of detail expected.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S3} §3.2
+G186 §3.2.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.10</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the role of Architecture Building Blocks (ABBs) and when they are used.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S4} §5.2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Briefly explain the guidelines and techniques that can be used during the Business Architecture phase:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S1} §4.5.3, 4.5.4, 4.5.5, 4.5.6, 4.5.7
+G178, G18A, G190, G206, G211</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Applying business capabilities</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Applying value streams</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Applying the organization map</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Applying information mapping</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Applying modeling techniques</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the technique of gap analysis and where it can be applied.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S2} §5.1, 5.2
+G186 §6.3.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how iteration can be used in architecture practices.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S3} §2.1
+G186 §5.2, 5.2.3</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe how the Implementation Factor Catalog can be used:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S2} §6.1</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Consolidated Gaps, Solutions, and Dependencies Matrix</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="TimesNewRoman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">·</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="10"/>
+        <color rgb="FF000000"/>
+        <rFont val="Times New Roman"/>
+        <family val="1"/>
+        <charset val="1"/>
+      </rPr>
+      <t xml:space="preserve">     Architecture Definition Increments Table</t>
+    </r>
+  </si>
+  <si>
+    <t xml:space="preserve">8.15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the need for a content metamodel/modeling and how it relates to the ACF.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S4} §1.2.1, 1.2.3
+G186 A</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain when the ACF needs to be filled throughout the ADM cycles.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S4} §1.3
+G186 E</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Describe the usage of an enterprise metamodel using the TOGAF Enterprise Metamodel as an example.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S4} §2.2</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain the use of a taxonomy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">8.19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Explain how risk assessment can be used.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">{S2} §9.4
+G152 §3.2.1, 5.3.4, 5.6.1, 5.7</t>
+  </si>
 </sst>
 </file>
 
@@ -1061,7 +2113,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="14">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1111,6 +2163,48 @@
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
+    <font>
+      <b val="true"/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="TimesNewRoman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="TimesNewRoman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <u val="single"/>
+      <sz val="12"/>
+      <color rgb="FF0563C1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="TimesNewRoman"/>
+      <family val="1"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="TimesNewRoman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="&#10;G186 §6.1.1, 6.1.2"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1122,11 +2216,11 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFE7E6E6"/>
-        <bgColor rgb="FFFFFFCC"/>
+        <bgColor rgb="FFDEEBF7"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="7">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -1155,8 +2249,29 @@
       <bottom style="thin"/>
       <diagonal/>
     </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom style="thin"/>
+      <diagonal/>
+    </border>
+    <border diagonalUp="false" diagonalDown="false">
+      <left style="thin"/>
+      <right style="thin"/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="20">
+  <cellStyleXfs count="21">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1180,8 +2295,11 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+    <xf numFmtId="164" fontId="10" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="36">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -1238,15 +2356,121 @@
       <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="11" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="12" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="4" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="8" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="2" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="7">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Comma" xfId="15" builtinId="3"/>
     <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
     <cellStyle name="Currency" xfId="17" builtinId="4"/>
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="*unknown*" xfId="20" builtinId="8"/>
   </cellStyles>
+  <dxfs count="1">
+    <dxf>
+      <font>
+        <name val="Arial"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <b val="0"/>
+        <i val="0"/>
+        <color rgb="FF0070C0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFDEEBF7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -1262,16 +2486,16 @@
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FF808000"/>
       <rgbColor rgb="FF800080"/>
-      <rgbColor rgb="FF008080"/>
+      <rgbColor rgb="FF0070C0"/>
       <rgbColor rgb="FFC0C0C0"/>
       <rgbColor rgb="FF808080"/>
       <rgbColor rgb="FF9999FF"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FFFFFFCC"/>
-      <rgbColor rgb="FFCCFFFF"/>
+      <rgbColor rgb="FFDEEBF7"/>
       <rgbColor rgb="FF660066"/>
       <rgbColor rgb="FFFF8080"/>
-      <rgbColor rgb="FF0066CC"/>
+      <rgbColor rgb="FF0563C1"/>
       <rgbColor rgb="FFCCCCFF"/>
       <rgbColor rgb="FF000080"/>
       <rgbColor rgb="FFFF00FF"/>
@@ -1317,8 +2541,8 @@
   </sheetPr>
   <dimension ref="A1:F114"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A72" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D84" activeCellId="0" sqref="D84"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C113" activeCellId="0" sqref="C113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3340,4 +4564,1813 @@
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:F121"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="F33" activeCellId="0" sqref="F33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="63.08"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="40.01"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="26.12"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="13.89"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="77.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.11"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A1" s="14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="15"/>
+      <c r="D1" s="16" t="s">
+        <v>323</v>
+      </c>
+      <c r="E1" s="17" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="17" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="14"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="16"/>
+      <c r="E2" s="18"/>
+      <c r="F2" s="18"/>
+    </row>
+    <row r="3" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A3" s="19" t="s">
+        <v>324</v>
+      </c>
+      <c r="B3" s="20" t="n">
+        <v>1.1</v>
+      </c>
+      <c r="C3" s="21" t="s">
+        <v>325</v>
+      </c>
+      <c r="D3" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E3" s="22" t="s">
+        <v>326</v>
+      </c>
+      <c r="F3" s="22" t="s">
+        <v>327</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="25.35" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A4" s="19"/>
+      <c r="B4" s="20" t="n">
+        <v>1.2</v>
+      </c>
+      <c r="C4" s="21" t="s">
+        <v>328</v>
+      </c>
+      <c r="D4" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="22" t="s">
+        <v>329</v>
+      </c>
+      <c r="F4" s="22" t="s">
+        <v>330</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A5" s="19"/>
+      <c r="B5" s="20" t="n">
+        <v>1.3</v>
+      </c>
+      <c r="C5" s="21" t="s">
+        <v>331</v>
+      </c>
+      <c r="D5" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E5" s="22" t="s">
+        <v>332</v>
+      </c>
+      <c r="F5" s="22" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="19"/>
+      <c r="B6" s="20"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="22"/>
+      <c r="E6" s="22"/>
+      <c r="F6" s="22"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A7" s="19"/>
+      <c r="B7" s="20" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="C7" s="21" t="s">
+        <v>334</v>
+      </c>
+      <c r="D7" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E7" s="22" t="s">
+        <v>335</v>
+      </c>
+      <c r="F7" s="22" t="s">
+        <v>336</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="19"/>
+      <c r="B8" s="20"/>
+      <c r="C8" s="21"/>
+      <c r="D8" s="22"/>
+      <c r="E8" s="22"/>
+      <c r="F8" s="22"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A9" s="19"/>
+      <c r="B9" s="20" t="n">
+        <v>1.5</v>
+      </c>
+      <c r="C9" s="23" t="s">
+        <v>337</v>
+      </c>
+      <c r="D9" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E9" s="22" t="s">
+        <v>338</v>
+      </c>
+      <c r="F9" s="22" t="s">
+        <v>339</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="54.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A10" s="19"/>
+      <c r="B10" s="20"/>
+      <c r="C10" s="23"/>
+      <c r="D10" s="22"/>
+      <c r="E10" s="22"/>
+      <c r="F10" s="22"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A11" s="19"/>
+      <c r="B11" s="20" t="n">
+        <v>1.6</v>
+      </c>
+      <c r="C11" s="21" t="s">
+        <v>340</v>
+      </c>
+      <c r="D11" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E11" s="22" t="s">
+        <v>341</v>
+      </c>
+      <c r="F11" s="22" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="30.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A12" s="19"/>
+      <c r="B12" s="20"/>
+      <c r="C12" s="21"/>
+      <c r="D12" s="22"/>
+      <c r="E12" s="22"/>
+      <c r="F12" s="22"/>
+    </row>
+    <row r="13" customFormat="false" ht="36.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A13" s="19"/>
+      <c r="B13" s="20" t="n">
+        <v>1.7</v>
+      </c>
+      <c r="C13" s="21" t="s">
+        <v>343</v>
+      </c>
+      <c r="D13" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="22" t="s">
+        <v>344</v>
+      </c>
+      <c r="F13" s="22" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="19"/>
+      <c r="B14" s="20" t="n">
+        <v>1.8</v>
+      </c>
+      <c r="C14" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="D14" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="22" t="s">
+        <v>347</v>
+      </c>
+      <c r="F14" s="22" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="19"/>
+      <c r="B15" s="20" t="n">
+        <v>1.9</v>
+      </c>
+      <c r="C15" s="21" t="s">
+        <v>349</v>
+      </c>
+      <c r="D15" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E15" s="22" t="s">
+        <v>350</v>
+      </c>
+      <c r="F15" s="22" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="46.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="19"/>
+      <c r="B16" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="21" t="s">
+        <v>352</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>353</v>
+      </c>
+      <c r="F16" s="22" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="97" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A17" s="19"/>
+      <c r="B17" s="20" t="n">
+        <v>1.11</v>
+      </c>
+      <c r="C17" s="21" t="s">
+        <v>355</v>
+      </c>
+      <c r="D17" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="22" t="s">
+        <v>356</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="37.3" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A18" s="19" t="s">
+        <v>358</v>
+      </c>
+      <c r="B18" s="20" t="n">
+        <v>2.1</v>
+      </c>
+      <c r="C18" s="21" t="s">
+        <v>359</v>
+      </c>
+      <c r="D18" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E18" s="22" t="s">
+        <v>361</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="19"/>
+      <c r="B19" s="20" t="n">
+        <v>2.2</v>
+      </c>
+      <c r="C19" s="21" t="s">
+        <v>363</v>
+      </c>
+      <c r="D19" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E19" s="22" t="s">
+        <v>364</v>
+      </c>
+      <c r="F19" s="22"/>
+    </row>
+    <row r="20" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="19"/>
+      <c r="B20" s="20" t="n">
+        <v>2.3</v>
+      </c>
+      <c r="C20" s="21" t="s">
+        <v>365</v>
+      </c>
+      <c r="D20" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E20" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="F20" s="22"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A21" s="19"/>
+      <c r="B21" s="20" t="n">
+        <v>2.4</v>
+      </c>
+      <c r="C21" s="21" t="s">
+        <v>366</v>
+      </c>
+      <c r="D21" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E21" s="25" t="s">
+        <v>367</v>
+      </c>
+      <c r="F21" s="25"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="19"/>
+      <c r="B22" s="20"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="24"/>
+      <c r="E22" s="25"/>
+      <c r="F22" s="25"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A23" s="19" t="s">
+        <v>368</v>
+      </c>
+      <c r="B23" s="20" t="n">
+        <v>3.1</v>
+      </c>
+      <c r="C23" s="21" t="s">
+        <v>369</v>
+      </c>
+      <c r="D23" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E23" s="22" t="s">
+        <v>370</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="50.7" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A24" s="19"/>
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="22"/>
+      <c r="F24" s="22"/>
+    </row>
+    <row r="25" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="19"/>
+      <c r="B25" s="20" t="n">
+        <v>3.2</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>372</v>
+      </c>
+      <c r="D25" s="26"/>
+      <c r="E25" s="26"/>
+      <c r="F25" s="22"/>
+    </row>
+    <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="19"/>
+      <c r="B26" s="20"/>
+      <c r="C26" s="27" t="s">
+        <v>373</v>
+      </c>
+      <c r="D26" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E26" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="F26" s="25" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="19"/>
+      <c r="B27" s="20"/>
+      <c r="C27" s="27" t="s">
+        <v>376</v>
+      </c>
+      <c r="D27" s="22"/>
+      <c r="E27" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="F27" s="28" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="19"/>
+      <c r="B28" s="20"/>
+      <c r="C28" s="27" t="s">
+        <v>378</v>
+      </c>
+      <c r="D28" s="22"/>
+      <c r="E28" s="22" t="s">
+        <v>374</v>
+      </c>
+      <c r="F28" s="29" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="19"/>
+      <c r="B29" s="20" t="n">
+        <v>3.3</v>
+      </c>
+      <c r="C29" s="21" t="s">
+        <v>380</v>
+      </c>
+      <c r="D29" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E29" s="22" t="s">
+        <v>381</v>
+      </c>
+      <c r="F29" s="22"/>
+    </row>
+    <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="19"/>
+      <c r="B30" s="20" t="n">
+        <v>3.4</v>
+      </c>
+      <c r="C30" s="21" t="s">
+        <v>382</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E30" s="22"/>
+      <c r="F30" s="22"/>
+    </row>
+    <row r="31" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="19"/>
+      <c r="B31" s="20"/>
+      <c r="C31" s="27" t="s">
+        <v>383</v>
+      </c>
+      <c r="D31" s="22"/>
+      <c r="E31" s="22" t="s">
+        <v>384</v>
+      </c>
+      <c r="F31" s="28" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="51.45" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A32" s="19"/>
+      <c r="B32" s="20"/>
+      <c r="C32" s="27" t="s">
+        <v>386</v>
+      </c>
+      <c r="D32" s="22"/>
+      <c r="E32" s="22" t="s">
+        <v>384</v>
+      </c>
+      <c r="F32" s="30" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="52.95" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A33" s="19"/>
+      <c r="B33" s="20"/>
+      <c r="C33" s="27" t="s">
+        <v>388</v>
+      </c>
+      <c r="D33" s="22"/>
+      <c r="E33" s="22" t="s">
+        <v>384</v>
+      </c>
+      <c r="F33" s="29" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A34" s="31" t="s">
+        <v>390</v>
+      </c>
+      <c r="B34" s="20" t="n">
+        <v>4.1</v>
+      </c>
+      <c r="C34" s="21" t="s">
+        <v>391</v>
+      </c>
+      <c r="D34" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="22" t="s">
+        <v>392</v>
+      </c>
+      <c r="F34" s="22"/>
+    </row>
+    <row r="35" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="31"/>
+      <c r="B35" s="20" t="n">
+        <v>4.2</v>
+      </c>
+      <c r="C35" s="21" t="s">
+        <v>393</v>
+      </c>
+      <c r="D35" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E35" s="22" t="s">
+        <v>394</v>
+      </c>
+      <c r="F35" s="22"/>
+    </row>
+    <row r="36" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A36" s="31"/>
+      <c r="B36" s="20" t="n">
+        <v>4.3</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>395</v>
+      </c>
+      <c r="D36" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E36" s="22" t="s">
+        <v>396</v>
+      </c>
+      <c r="F36" s="22"/>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="31"/>
+      <c r="B37" s="20"/>
+      <c r="C37" s="27" t="s">
+        <v>397</v>
+      </c>
+      <c r="D37" s="24"/>
+      <c r="E37" s="22"/>
+      <c r="F37" s="28"/>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="31"/>
+      <c r="B38" s="20"/>
+      <c r="C38" s="27" t="s">
+        <v>398</v>
+      </c>
+      <c r="D38" s="24"/>
+      <c r="E38" s="22"/>
+      <c r="F38" s="28"/>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="31"/>
+      <c r="B39" s="20"/>
+      <c r="C39" s="27" t="s">
+        <v>399</v>
+      </c>
+      <c r="D39" s="24"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="29"/>
+    </row>
+    <row r="40" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A40" s="31"/>
+      <c r="B40" s="20" t="n">
+        <v>4.4</v>
+      </c>
+      <c r="C40" s="32" t="s">
+        <v>400</v>
+      </c>
+      <c r="D40" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E40" s="22" t="s">
+        <v>401</v>
+      </c>
+      <c r="F40" s="22"/>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="31"/>
+      <c r="B41" s="20"/>
+      <c r="C41" s="33"/>
+      <c r="D41" s="24"/>
+      <c r="E41" s="22"/>
+      <c r="F41" s="29"/>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A42" s="31"/>
+      <c r="B42" s="20" t="n">
+        <v>4.5</v>
+      </c>
+      <c r="C42" s="22" t="s">
+        <v>402</v>
+      </c>
+      <c r="D42" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E42" s="22" t="s">
+        <v>403</v>
+      </c>
+      <c r="F42" s="22"/>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="31"/>
+      <c r="B43" s="20"/>
+      <c r="C43" s="22"/>
+      <c r="D43" s="24"/>
+      <c r="E43" s="22"/>
+      <c r="F43" s="29"/>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A44" s="31"/>
+      <c r="B44" s="20" t="n">
+        <v>4.6</v>
+      </c>
+      <c r="C44" s="29" t="s">
+        <v>404</v>
+      </c>
+      <c r="D44" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E44" s="29" t="s">
+        <v>405</v>
+      </c>
+      <c r="F44" s="29"/>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="31"/>
+      <c r="B45" s="20"/>
+      <c r="C45" s="29"/>
+      <c r="D45" s="24"/>
+      <c r="E45" s="29"/>
+      <c r="F45" s="29"/>
+    </row>
+    <row r="46" customFormat="false" ht="35.05" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A46" s="31"/>
+      <c r="B46" s="20" t="n">
+        <v>4.7</v>
+      </c>
+      <c r="C46" s="32" t="s">
+        <v>406</v>
+      </c>
+      <c r="D46" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>407</v>
+      </c>
+      <c r="F46" s="22"/>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="31"/>
+      <c r="B47" s="20"/>
+      <c r="C47" s="33"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="22"/>
+      <c r="F47" s="29"/>
+    </row>
+    <row r="48" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A48" s="31"/>
+      <c r="B48" s="20" t="n">
+        <v>4.8</v>
+      </c>
+      <c r="C48" s="25" t="s">
+        <v>408</v>
+      </c>
+      <c r="D48" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E48" s="22" t="s">
+        <v>409</v>
+      </c>
+      <c r="F48" s="22"/>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="31"/>
+      <c r="B49" s="20"/>
+      <c r="C49" s="29"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="22"/>
+      <c r="F49" s="29"/>
+    </row>
+    <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A50" s="31"/>
+      <c r="B50" s="20" t="n">
+        <v>4.9</v>
+      </c>
+      <c r="C50" s="25" t="s">
+        <v>410</v>
+      </c>
+      <c r="D50" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E50" s="22" t="s">
+        <v>411</v>
+      </c>
+      <c r="F50" s="22"/>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="31"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="29"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="22"/>
+      <c r="F51" s="29"/>
+    </row>
+    <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A52" s="19" t="s">
+        <v>412</v>
+      </c>
+      <c r="B52" s="20" t="n">
+        <v>5.1</v>
+      </c>
+      <c r="C52" s="21" t="s">
+        <v>413</v>
+      </c>
+      <c r="D52" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E52" s="22" t="s">
+        <v>414</v>
+      </c>
+      <c r="F52" s="22"/>
+    </row>
+    <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="19"/>
+      <c r="B53" s="20" t="n">
+        <v>5.2</v>
+      </c>
+      <c r="C53" s="21" t="s">
+        <v>415</v>
+      </c>
+      <c r="D53" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E53" s="22" t="s">
+        <v>416</v>
+      </c>
+      <c r="F53" s="22"/>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="19"/>
+      <c r="B54" s="20" t="n">
+        <v>5.3</v>
+      </c>
+      <c r="C54" s="21" t="s">
+        <v>417</v>
+      </c>
+      <c r="D54" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E54" s="22" t="s">
+        <v>418</v>
+      </c>
+      <c r="F54" s="22"/>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="19"/>
+      <c r="B55" s="20" t="n">
+        <v>5.4</v>
+      </c>
+      <c r="C55" s="21" t="s">
+        <v>419</v>
+      </c>
+      <c r="D55" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E55" s="22" t="s">
+        <v>416</v>
+      </c>
+      <c r="F55" s="22"/>
+    </row>
+    <row r="56" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="19"/>
+      <c r="B56" s="20" t="n">
+        <v>5.5</v>
+      </c>
+      <c r="C56" s="21" t="s">
+        <v>420</v>
+      </c>
+      <c r="D56" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E56" s="22" t="s">
+        <v>416</v>
+      </c>
+      <c r="F56" s="22"/>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A57" s="19"/>
+      <c r="B57" s="20" t="n">
+        <v>5.6</v>
+      </c>
+      <c r="C57" s="21" t="s">
+        <v>421</v>
+      </c>
+      <c r="D57" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E57" s="22" t="s">
+        <v>422</v>
+      </c>
+      <c r="F57" s="22"/>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="19"/>
+      <c r="B58" s="20"/>
+      <c r="C58" s="21"/>
+      <c r="D58" s="24"/>
+      <c r="E58" s="22"/>
+      <c r="F58" s="29"/>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A59" s="19"/>
+      <c r="B59" s="20" t="n">
+        <v>5.7</v>
+      </c>
+      <c r="C59" s="21" t="s">
+        <v>423</v>
+      </c>
+      <c r="D59" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E59" s="22" t="s">
+        <v>424</v>
+      </c>
+      <c r="F59" s="22"/>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="19"/>
+      <c r="B60" s="20"/>
+      <c r="C60" s="21"/>
+      <c r="D60" s="24"/>
+      <c r="E60" s="22"/>
+      <c r="F60" s="29"/>
+    </row>
+    <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="19"/>
+      <c r="B61" s="20" t="n">
+        <v>5.8</v>
+      </c>
+      <c r="C61" s="21" t="s">
+        <v>425</v>
+      </c>
+      <c r="D61" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E61" s="22" t="s">
+        <v>426</v>
+      </c>
+      <c r="F61" s="22"/>
+    </row>
+    <row r="62" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="19"/>
+      <c r="B62" s="20" t="n">
+        <v>5.9</v>
+      </c>
+      <c r="C62" s="21" t="s">
+        <v>427</v>
+      </c>
+      <c r="D62" s="24" t="s">
+        <v>7</v>
+      </c>
+      <c r="E62" s="22" t="s">
+        <v>428</v>
+      </c>
+      <c r="F62" s="22"/>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A63" s="19"/>
+      <c r="B63" s="20" t="s">
+        <v>429</v>
+      </c>
+      <c r="C63" s="21" t="s">
+        <v>430</v>
+      </c>
+      <c r="D63" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E63" s="22" t="s">
+        <v>431</v>
+      </c>
+      <c r="F63" s="22"/>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="19"/>
+      <c r="B64" s="20"/>
+      <c r="C64" s="21"/>
+      <c r="D64" s="24"/>
+      <c r="E64" s="22"/>
+      <c r="F64" s="29"/>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="19"/>
+      <c r="B65" s="20" t="n">
+        <v>5.11</v>
+      </c>
+      <c r="C65" s="21" t="s">
+        <v>432</v>
+      </c>
+      <c r="D65" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E65" s="22" t="s">
+        <v>433</v>
+      </c>
+      <c r="F65" s="22"/>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A66" s="19"/>
+      <c r="B66" s="20" t="n">
+        <v>5.12</v>
+      </c>
+      <c r="C66" s="21" t="s">
+        <v>434</v>
+      </c>
+      <c r="D66" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E66" s="22" t="s">
+        <v>435</v>
+      </c>
+      <c r="F66" s="22"/>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="19"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="24"/>
+      <c r="E67" s="22"/>
+      <c r="F67" s="29"/>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A68" s="19"/>
+      <c r="B68" s="20" t="n">
+        <v>5.13</v>
+      </c>
+      <c r="C68" s="21" t="s">
+        <v>436</v>
+      </c>
+      <c r="D68" s="24" t="s">
+        <v>11</v>
+      </c>
+      <c r="E68" s="22" t="s">
+        <v>437</v>
+      </c>
+      <c r="F68" s="22"/>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="19"/>
+      <c r="B69" s="20"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="24"/>
+      <c r="E69" s="22"/>
+      <c r="F69" s="29"/>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A70" s="19"/>
+      <c r="B70" s="20" t="n">
+        <v>5.14</v>
+      </c>
+      <c r="C70" s="21" t="s">
+        <v>438</v>
+      </c>
+      <c r="D70" s="24" t="s">
+        <v>360</v>
+      </c>
+      <c r="E70" s="22" t="s">
+        <v>439</v>
+      </c>
+      <c r="F70" s="22"/>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="19"/>
+      <c r="B71" s="20"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="24"/>
+      <c r="E71" s="22"/>
+      <c r="F71" s="29"/>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="19"/>
+      <c r="B72" s="20" t="n">
+        <v>5.15</v>
+      </c>
+      <c r="C72" s="21" t="s">
+        <v>440</v>
+      </c>
+      <c r="D72" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E72" s="22" t="s">
+        <v>441</v>
+      </c>
+      <c r="F72" s="22"/>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A73" s="34" t="s">
+        <v>442</v>
+      </c>
+      <c r="B73" s="20" t="n">
+        <v>6.1</v>
+      </c>
+      <c r="C73" s="32" t="s">
+        <v>443</v>
+      </c>
+      <c r="D73" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E73" s="22" t="s">
+        <v>444</v>
+      </c>
+      <c r="F73" s="22"/>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="34"/>
+      <c r="B74" s="20"/>
+      <c r="C74" s="35" t="s">
+        <v>445</v>
+      </c>
+      <c r="D74" s="22"/>
+      <c r="E74" s="22"/>
+      <c r="F74" s="29"/>
+    </row>
+    <row r="75" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A75" s="34"/>
+      <c r="B75" s="20" t="n">
+        <v>6.2</v>
+      </c>
+      <c r="C75" s="21" t="s">
+        <v>446</v>
+      </c>
+      <c r="D75" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E75" s="25" t="s">
+        <v>447</v>
+      </c>
+      <c r="F75" s="25"/>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="34"/>
+      <c r="B76" s="20"/>
+      <c r="C76" s="21"/>
+      <c r="D76" s="22"/>
+      <c r="E76" s="29"/>
+      <c r="F76" s="29"/>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A77" s="34"/>
+      <c r="B77" s="20" t="n">
+        <v>6.3</v>
+      </c>
+      <c r="C77" s="21" t="s">
+        <v>448</v>
+      </c>
+      <c r="D77" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E77" s="22" t="s">
+        <v>449</v>
+      </c>
+      <c r="F77" s="22"/>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="34"/>
+      <c r="B78" s="20"/>
+      <c r="C78" s="21"/>
+      <c r="D78" s="22"/>
+      <c r="E78" s="22"/>
+      <c r="F78" s="29"/>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A79" s="19" t="s">
+        <v>450</v>
+      </c>
+      <c r="B79" s="20" t="n">
+        <v>7.1</v>
+      </c>
+      <c r="C79" s="21" t="s">
+        <v>451</v>
+      </c>
+      <c r="D79" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E79" s="22" t="s">
+        <v>452</v>
+      </c>
+      <c r="F79" s="22"/>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="19"/>
+      <c r="B80" s="20"/>
+      <c r="C80" s="21"/>
+      <c r="D80" s="22"/>
+      <c r="E80" s="22"/>
+      <c r="F80" s="29"/>
+    </row>
+    <row r="81" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="19"/>
+      <c r="B81" s="20" t="n">
+        <v>7.2</v>
+      </c>
+      <c r="C81" s="21" t="s">
+        <v>453</v>
+      </c>
+      <c r="D81" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E81" s="22" t="s">
+        <v>454</v>
+      </c>
+      <c r="F81" s="22"/>
+    </row>
+    <row r="82" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="19"/>
+      <c r="B82" s="20" t="n">
+        <v>7.3</v>
+      </c>
+      <c r="C82" s="21" t="s">
+        <v>455</v>
+      </c>
+      <c r="D82" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E82" s="22" t="s">
+        <v>456</v>
+      </c>
+      <c r="F82" s="22"/>
+    </row>
+    <row r="83" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A83" s="19" t="s">
+        <v>457</v>
+      </c>
+      <c r="B83" s="20" t="n">
+        <v>8.1</v>
+      </c>
+      <c r="C83" s="21" t="s">
+        <v>458</v>
+      </c>
+      <c r="D83" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E83" s="22" t="s">
+        <v>459</v>
+      </c>
+      <c r="F83" s="22"/>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="19"/>
+      <c r="B84" s="20" t="n">
+        <v>8.2</v>
+      </c>
+      <c r="C84" s="21" t="s">
+        <v>460</v>
+      </c>
+      <c r="D84" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E84" s="22" t="s">
+        <v>461</v>
+      </c>
+      <c r="F84" s="22"/>
+    </row>
+    <row r="85" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A85" s="19"/>
+      <c r="B85" s="20" t="n">
+        <v>8.3</v>
+      </c>
+      <c r="C85" s="21" t="s">
+        <v>462</v>
+      </c>
+      <c r="D85" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E85" s="22" t="s">
+        <v>463</v>
+      </c>
+      <c r="F85" s="22"/>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="19"/>
+      <c r="B86" s="20"/>
+      <c r="C86" s="21"/>
+      <c r="D86" s="22"/>
+      <c r="E86" s="22"/>
+      <c r="F86" s="22"/>
+    </row>
+    <row r="87" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="19"/>
+      <c r="B87" s="20" t="n">
+        <v>8.4</v>
+      </c>
+      <c r="C87" s="21" t="s">
+        <v>464</v>
+      </c>
+      <c r="D87" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E87" s="22" t="s">
+        <v>465</v>
+      </c>
+      <c r="F87" s="22"/>
+    </row>
+    <row r="88" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A88" s="19"/>
+      <c r="B88" s="20" t="n">
+        <v>8.5</v>
+      </c>
+      <c r="C88" s="21" t="s">
+        <v>466</v>
+      </c>
+      <c r="D88" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E88" s="22" t="s">
+        <v>467</v>
+      </c>
+      <c r="F88" s="22"/>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="19"/>
+      <c r="B89" s="20"/>
+      <c r="C89" s="27" t="s">
+        <v>468</v>
+      </c>
+      <c r="D89" s="22"/>
+      <c r="E89" s="22"/>
+      <c r="F89" s="22"/>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="19"/>
+      <c r="B90" s="20"/>
+      <c r="C90" s="27" t="s">
+        <v>469</v>
+      </c>
+      <c r="D90" s="22"/>
+      <c r="E90" s="22"/>
+      <c r="F90" s="22"/>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="19"/>
+      <c r="B91" s="20"/>
+      <c r="C91" s="27" t="s">
+        <v>470</v>
+      </c>
+      <c r="D91" s="22"/>
+      <c r="E91" s="22"/>
+      <c r="F91" s="22"/>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="19"/>
+      <c r="B92" s="20"/>
+      <c r="C92" s="27" t="s">
+        <v>471</v>
+      </c>
+      <c r="D92" s="22"/>
+      <c r="E92" s="22"/>
+      <c r="F92" s="22"/>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="19"/>
+      <c r="B93" s="20"/>
+      <c r="C93" s="27" t="s">
+        <v>472</v>
+      </c>
+      <c r="D93" s="22"/>
+      <c r="E93" s="22"/>
+      <c r="F93" s="22"/>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="19"/>
+      <c r="B94" s="20"/>
+      <c r="C94" s="27" t="s">
+        <v>473</v>
+      </c>
+      <c r="D94" s="22"/>
+      <c r="E94" s="22"/>
+      <c r="F94" s="22"/>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="19"/>
+      <c r="B95" s="20"/>
+      <c r="C95" s="27" t="s">
+        <v>474</v>
+      </c>
+      <c r="D95" s="22"/>
+      <c r="E95" s="22"/>
+      <c r="F95" s="22"/>
+    </row>
+    <row r="96" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="19"/>
+      <c r="B96" s="20" t="n">
+        <v>8.6</v>
+      </c>
+      <c r="C96" s="21" t="s">
+        <v>475</v>
+      </c>
+      <c r="D96" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E96" s="22" t="s">
+        <v>476</v>
+      </c>
+      <c r="F96" s="22"/>
+    </row>
+    <row r="97" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="19"/>
+      <c r="B97" s="20" t="n">
+        <v>8.7</v>
+      </c>
+      <c r="C97" s="21" t="s">
+        <v>477</v>
+      </c>
+      <c r="D97" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E97" s="22" t="s">
+        <v>478</v>
+      </c>
+      <c r="F97" s="22"/>
+    </row>
+    <row r="98" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="19"/>
+      <c r="B98" s="20" t="n">
+        <v>8.8</v>
+      </c>
+      <c r="C98" s="21" t="s">
+        <v>479</v>
+      </c>
+      <c r="D98" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E98" s="22" t="s">
+        <v>237</v>
+      </c>
+      <c r="F98" s="22"/>
+    </row>
+    <row r="99" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A99" s="19"/>
+      <c r="B99" s="20" t="n">
+        <v>8.9</v>
+      </c>
+      <c r="C99" s="21" t="s">
+        <v>480</v>
+      </c>
+      <c r="D99" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E99" s="22" t="s">
+        <v>481</v>
+      </c>
+      <c r="F99" s="22"/>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="19"/>
+      <c r="B100" s="20"/>
+      <c r="C100" s="21"/>
+      <c r="D100" s="22"/>
+      <c r="E100" s="22"/>
+      <c r="F100" s="22"/>
+    </row>
+    <row r="101" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A101" s="19"/>
+      <c r="B101" s="20" t="s">
+        <v>482</v>
+      </c>
+      <c r="C101" s="21" t="s">
+        <v>483</v>
+      </c>
+      <c r="D101" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E101" s="22" t="s">
+        <v>484</v>
+      </c>
+      <c r="F101" s="22"/>
+    </row>
+    <row r="102" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A102" s="19"/>
+      <c r="B102" s="20" t="n">
+        <v>8.11</v>
+      </c>
+      <c r="C102" s="21" t="s">
+        <v>485</v>
+      </c>
+      <c r="D102" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E102" s="22" t="s">
+        <v>486</v>
+      </c>
+      <c r="F102" s="22"/>
+    </row>
+    <row r="103" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A103" s="19"/>
+      <c r="B103" s="20"/>
+      <c r="C103" s="27" t="s">
+        <v>487</v>
+      </c>
+      <c r="D103" s="22"/>
+      <c r="E103" s="22"/>
+      <c r="F103" s="22"/>
+    </row>
+    <row r="104" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A104" s="19"/>
+      <c r="B104" s="20"/>
+      <c r="C104" s="27" t="s">
+        <v>488</v>
+      </c>
+      <c r="D104" s="22"/>
+      <c r="E104" s="22"/>
+      <c r="F104" s="22"/>
+    </row>
+    <row r="105" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A105" s="19"/>
+      <c r="B105" s="20"/>
+      <c r="C105" s="27" t="s">
+        <v>489</v>
+      </c>
+      <c r="D105" s="22"/>
+      <c r="E105" s="22"/>
+      <c r="F105" s="22"/>
+    </row>
+    <row r="106" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A106" s="19"/>
+      <c r="B106" s="20"/>
+      <c r="C106" s="27" t="s">
+        <v>490</v>
+      </c>
+      <c r="D106" s="22"/>
+      <c r="E106" s="22"/>
+      <c r="F106" s="22"/>
+    </row>
+    <row r="107" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A107" s="19"/>
+      <c r="B107" s="20"/>
+      <c r="C107" s="27" t="s">
+        <v>491</v>
+      </c>
+      <c r="D107" s="22"/>
+      <c r="E107" s="22"/>
+      <c r="F107" s="22"/>
+    </row>
+    <row r="108" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A108" s="19"/>
+      <c r="B108" s="20" t="n">
+        <v>8.12</v>
+      </c>
+      <c r="C108" s="21" t="s">
+        <v>492</v>
+      </c>
+      <c r="D108" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E108" s="22" t="s">
+        <v>493</v>
+      </c>
+      <c r="F108" s="22"/>
+    </row>
+    <row r="109" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A109" s="19"/>
+      <c r="B109" s="20"/>
+      <c r="C109" s="21"/>
+      <c r="D109" s="22"/>
+      <c r="E109" s="22"/>
+      <c r="F109" s="22"/>
+    </row>
+    <row r="110" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A110" s="19"/>
+      <c r="B110" s="20" t="n">
+        <v>8.13</v>
+      </c>
+      <c r="C110" s="21" t="s">
+        <v>494</v>
+      </c>
+      <c r="D110" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E110" s="22" t="s">
+        <v>495</v>
+      </c>
+      <c r="F110" s="22"/>
+    </row>
+    <row r="111" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A111" s="19"/>
+      <c r="B111" s="20"/>
+      <c r="C111" s="21"/>
+      <c r="D111" s="22"/>
+      <c r="E111" s="22"/>
+      <c r="F111" s="22"/>
+    </row>
+    <row r="112" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A112" s="19"/>
+      <c r="B112" s="20" t="n">
+        <v>8.14</v>
+      </c>
+      <c r="C112" s="21" t="s">
+        <v>496</v>
+      </c>
+      <c r="D112" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E112" s="22" t="s">
+        <v>497</v>
+      </c>
+      <c r="F112" s="22"/>
+    </row>
+    <row r="113" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A113" s="19"/>
+      <c r="B113" s="20"/>
+      <c r="C113" s="27" t="s">
+        <v>498</v>
+      </c>
+      <c r="D113" s="22"/>
+      <c r="E113" s="22"/>
+      <c r="F113" s="22"/>
+    </row>
+    <row r="114" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A114" s="19"/>
+      <c r="B114" s="20"/>
+      <c r="C114" s="27" t="s">
+        <v>499</v>
+      </c>
+      <c r="D114" s="22"/>
+      <c r="E114" s="22"/>
+      <c r="F114" s="22"/>
+    </row>
+    <row r="115" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A115" s="19"/>
+      <c r="B115" s="20" t="s">
+        <v>500</v>
+      </c>
+      <c r="C115" s="21" t="s">
+        <v>501</v>
+      </c>
+      <c r="D115" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E115" s="22" t="s">
+        <v>502</v>
+      </c>
+      <c r="F115" s="22"/>
+    </row>
+    <row r="116" customFormat="false" ht="32.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A116" s="19"/>
+      <c r="B116" s="20"/>
+      <c r="C116" s="21"/>
+      <c r="D116" s="22"/>
+      <c r="E116" s="22"/>
+      <c r="F116" s="22"/>
+    </row>
+    <row r="117" customFormat="false" ht="23.85" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+      <c r="A117" s="19"/>
+      <c r="B117" s="20" t="s">
+        <v>503</v>
+      </c>
+      <c r="C117" s="21" t="s">
+        <v>504</v>
+      </c>
+      <c r="D117" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E117" s="22" t="s">
+        <v>505</v>
+      </c>
+      <c r="F117" s="22"/>
+    </row>
+    <row r="118" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A118" s="19"/>
+      <c r="B118" s="20"/>
+      <c r="C118" s="21"/>
+      <c r="D118" s="22"/>
+      <c r="E118" s="22"/>
+      <c r="F118" s="22"/>
+    </row>
+    <row r="119" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A119" s="19"/>
+      <c r="B119" s="20" t="s">
+        <v>506</v>
+      </c>
+      <c r="C119" s="21" t="s">
+        <v>507</v>
+      </c>
+      <c r="D119" s="22" t="s">
+        <v>7</v>
+      </c>
+      <c r="E119" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="F119" s="22"/>
+    </row>
+    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A120" s="19"/>
+      <c r="B120" s="20" t="s">
+        <v>509</v>
+      </c>
+      <c r="C120" s="21" t="s">
+        <v>510</v>
+      </c>
+      <c r="D120" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E120" s="22" t="s">
+        <v>508</v>
+      </c>
+      <c r="F120" s="22"/>
+    </row>
+    <row r="121" customFormat="false" ht="35.05" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A121" s="19"/>
+      <c r="B121" s="20" t="s">
+        <v>511</v>
+      </c>
+      <c r="C121" s="21" t="s">
+        <v>512</v>
+      </c>
+      <c r="D121" s="22" t="s">
+        <v>11</v>
+      </c>
+      <c r="E121" s="22" t="s">
+        <v>513</v>
+      </c>
+      <c r="F121" s="22"/>
+    </row>
+  </sheetData>
+  <mergeCells count="131">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="B1:C2"/>
+    <mergeCell ref="D1:D2"/>
+    <mergeCell ref="A3:A17"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="D5:D6"/>
+    <mergeCell ref="E5:E6"/>
+    <mergeCell ref="F5:F6"/>
+    <mergeCell ref="B7:B8"/>
+    <mergeCell ref="C7:C8"/>
+    <mergeCell ref="D7:D8"/>
+    <mergeCell ref="E7:E8"/>
+    <mergeCell ref="F7:F8"/>
+    <mergeCell ref="B9:B10"/>
+    <mergeCell ref="C9:C10"/>
+    <mergeCell ref="D9:D10"/>
+    <mergeCell ref="E9:E10"/>
+    <mergeCell ref="F9:F10"/>
+    <mergeCell ref="B11:B12"/>
+    <mergeCell ref="C11:C12"/>
+    <mergeCell ref="D11:D12"/>
+    <mergeCell ref="E11:E12"/>
+    <mergeCell ref="F11:F12"/>
+    <mergeCell ref="A18:A22"/>
+    <mergeCell ref="B21:B22"/>
+    <mergeCell ref="C21:C22"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="F21:F22"/>
+    <mergeCell ref="A23:A33"/>
+    <mergeCell ref="B23:B24"/>
+    <mergeCell ref="C23:C24"/>
+    <mergeCell ref="D23:D24"/>
+    <mergeCell ref="E23:E24"/>
+    <mergeCell ref="F23:F24"/>
+    <mergeCell ref="B25:B28"/>
+    <mergeCell ref="B30:B33"/>
+    <mergeCell ref="A34:A51"/>
+    <mergeCell ref="B36:B39"/>
+    <mergeCell ref="D36:D39"/>
+    <mergeCell ref="E36:E39"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="E40:E41"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="C42:C43"/>
+    <mergeCell ref="D42:D43"/>
+    <mergeCell ref="E42:E43"/>
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="C44:C45"/>
+    <mergeCell ref="D44:D45"/>
+    <mergeCell ref="E44:E45"/>
+    <mergeCell ref="B46:B47"/>
+    <mergeCell ref="D46:D47"/>
+    <mergeCell ref="E46:E47"/>
+    <mergeCell ref="B48:B49"/>
+    <mergeCell ref="D48:D49"/>
+    <mergeCell ref="E48:E49"/>
+    <mergeCell ref="B50:B51"/>
+    <mergeCell ref="D50:D51"/>
+    <mergeCell ref="E50:E51"/>
+    <mergeCell ref="A52:A72"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="D57:D58"/>
+    <mergeCell ref="E57:E58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="D59:D60"/>
+    <mergeCell ref="E59:E60"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="D63:D64"/>
+    <mergeCell ref="E63:E64"/>
+    <mergeCell ref="B66:B67"/>
+    <mergeCell ref="C66:C67"/>
+    <mergeCell ref="D66:D67"/>
+    <mergeCell ref="E66:E67"/>
+    <mergeCell ref="B68:B69"/>
+    <mergeCell ref="C68:C69"/>
+    <mergeCell ref="D68:D69"/>
+    <mergeCell ref="E68:E69"/>
+    <mergeCell ref="B70:B71"/>
+    <mergeCell ref="C70:C71"/>
+    <mergeCell ref="D70:D71"/>
+    <mergeCell ref="E70:E71"/>
+    <mergeCell ref="A73:A78"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="D73:D74"/>
+    <mergeCell ref="E73:E74"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="D77:D78"/>
+    <mergeCell ref="E77:E78"/>
+    <mergeCell ref="A79:A82"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="D79:D80"/>
+    <mergeCell ref="E79:E80"/>
+    <mergeCell ref="A83:A121"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="D85:D86"/>
+    <mergeCell ref="B88:B95"/>
+    <mergeCell ref="D88:D95"/>
+    <mergeCell ref="E88:E95"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="B102:B107"/>
+    <mergeCell ref="D102:D107"/>
+    <mergeCell ref="E102:E107"/>
+    <mergeCell ref="B108:B109"/>
+    <mergeCell ref="C108:C109"/>
+    <mergeCell ref="D108:D109"/>
+    <mergeCell ref="E108:E109"/>
+    <mergeCell ref="B110:B111"/>
+    <mergeCell ref="C110:C111"/>
+    <mergeCell ref="D110:D111"/>
+    <mergeCell ref="E110:E111"/>
+    <mergeCell ref="B112:B114"/>
+    <mergeCell ref="D112:D114"/>
+    <mergeCell ref="E112:E114"/>
+    <mergeCell ref="B115:B116"/>
+    <mergeCell ref="C115:C116"/>
+    <mergeCell ref="D115:D116"/>
+    <mergeCell ref="E115:E116"/>
+    <mergeCell ref="B117:B118"/>
+    <mergeCell ref="C117:C118"/>
+    <mergeCell ref="D117:D118"/>
+  </mergeCells>
+  <conditionalFormatting sqref="D72:D121 D19 D22 D24 D27:D29 D31:D35 D1:D17">
+    <cfRule type="containsText" priority="2" operator="containsText" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="3_Applying" dxfId="0">
+      <formula>NOT(ISERROR(SEARCH("3_Applying",D1)))</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <hyperlinks>
+    <hyperlink ref="F3" r:id="rId1" location="_Toc95288808" display="https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_3.html#_Toc95288808"/>
+    <hyperlink ref="F4" r:id="rId2" location="_Toc95288812" display="https://pubs.opengroup.org/togaf-standard/adm-practitioners/adm-practitioners_3.html#_Toc95288812"/>
+    <hyperlink ref="F14" r:id="rId3" location="_Toc95208526" display="https://pubs.opengroup.org/togaf-standard/integrating-risk-and-security/integrating-risk-and-security_1.html#_Toc95208526"/>
+    <hyperlink ref="F15" r:id="rId4" location="_Toc95208548" display="https://pubs.opengroup.org/togaf-standard/integrating-risk-and-security/integrating-risk-and-security_4.html#_Toc95208548"/>
+    <hyperlink ref="F16" r:id="rId5" location="_Toc95208541" display="https://pubs.opengroup.org/togaf-standard/integrating-risk-and-security/integrating-risk-and-security_3.html#_Toc95208541"/>
+  </hyperlinks>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>